<commit_message>
edited for grid search
</commit_message>
<xml_diff>
--- a/models/Regression models heatmap with mean(ordered) with hyper(version 4).xlsx
+++ b/models/Regression models heatmap with mean(ordered) with hyper(version 4).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vichu\Downloads\90106\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2B4D865D-1973-49C9-B493-D1DD73630642}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA0A370-7157-446C-9617-CD09FE6C1FBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-8670" yWindow="6030" windowWidth="17280" windowHeight="9420" activeTab="1" xr2:uid="{9A6EADF9-FE04-4789-B7ED-5E14F238B3D0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{9A6EADF9-FE04-4789-B7ED-5E14F238B3D0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="184" uniqueCount="53">
   <si>
     <t>Merriwa</t>
   </si>
@@ -249,523 +249,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="108">
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00CC66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFCC99"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF6600"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF99FF66"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="36">
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
       <fill>
@@ -1351,8 +835,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AE61"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="P62" sqref="P62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3405,100 +2889,100 @@
       <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:16" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="D44" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C44" s="2" t="s">
+      <c r="E44" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="2" t="s">
+      <c r="F44" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E44" s="2" t="s">
+      <c r="G44" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="2" t="s">
+      <c r="H44" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="G44" s="2" t="s">
+      <c r="I44" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="H44" s="2" t="s">
+      <c r="J44" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="I44" s="2" t="s">
+      <c r="K44" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="J44" s="2" t="s">
+      <c r="L44" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="K44" s="2" t="s">
+      <c r="M44" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="L44" s="2" t="s">
+      <c r="N44" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="M44" s="2" t="s">
+      <c r="O44" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="N44" s="2" t="s">
+      <c r="P44" s="2" t="s">
         <v>48</v>
-      </c>
-      <c r="O44" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="P44" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B45">
+      <c r="B45" s="3">
+        <v>0.83320000000000005</v>
+      </c>
+      <c r="C45" s="3">
+        <v>0.71511999999999998</v>
+      </c>
+      <c r="D45">
         <v>0.87641999999999998</v>
       </c>
-      <c r="C45">
-        <v>0.87295999999999996</v>
-      </c>
-      <c r="D45" s="3">
-        <v>0.88249</v>
-      </c>
-      <c r="E45" s="3">
-        <v>0.87692000000000003</v>
+      <c r="E45">
+        <v>0.87553999999999998</v>
       </c>
       <c r="F45" s="3">
+        <v>0.92301</v>
+      </c>
+      <c r="G45" s="3">
+        <v>0.93095000000000006</v>
+      </c>
+      <c r="H45" s="3">
         <v>0.85182999999999998</v>
       </c>
-      <c r="G45" s="3">
-        <v>0.79551000000000005</v>
-      </c>
-      <c r="H45" s="3">
-        <v>0.53876999999999997</v>
-      </c>
       <c r="I45" s="3">
+        <v>0.82586999999999999</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0.74636000000000002</v>
+      </c>
+      <c r="K45" s="3">
         <v>0.88599000000000006</v>
       </c>
-      <c r="J45" s="3">
-        <v>0.88683999999999996</v>
-      </c>
-      <c r="K45" s="3">
-        <v>0.92549000000000003</v>
-      </c>
       <c r="L45" s="3">
-        <v>0.92301999999999995</v>
+        <v>0.88632999999999995</v>
       </c>
       <c r="M45" s="3">
+        <v>0.92554000000000003</v>
+      </c>
+      <c r="N45" s="3">
+        <v>0.92303000000000002</v>
+      </c>
+      <c r="O45" s="3">
         <v>0.83567000000000002</v>
       </c>
-      <c r="N45" s="3">
-        <v>0.83565999999999996</v>
-      </c>
-      <c r="O45" s="3">
-        <v>0.83320000000000005</v>
-      </c>
       <c r="P45" s="3">
-        <v>0.71511999999999998</v>
+        <v>0.83567999999999998</v>
       </c>
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.3">
@@ -3506,49 +2990,49 @@
         <v>2</v>
       </c>
       <c r="B46">
+        <v>212.95909</v>
+      </c>
+      <c r="C46">
+        <v>318.60122000000001</v>
+      </c>
+      <c r="D46">
         <v>171.77404000000001</v>
       </c>
-      <c r="C46">
-        <v>172.24589</v>
-      </c>
-      <c r="D46">
-        <v>188.35473999999999</v>
-      </c>
       <c r="E46">
-        <v>177.00949</v>
+        <v>170.69199</v>
       </c>
       <c r="F46">
+        <v>124.89474</v>
+      </c>
+      <c r="G46">
+        <v>136.5179</v>
+      </c>
+      <c r="H46">
         <v>172.38102000000001</v>
       </c>
-      <c r="G46">
-        <v>250.54906</v>
-      </c>
-      <c r="H46">
-        <v>238.25982999999999</v>
-      </c>
       <c r="I46">
-        <v>170.48398</v>
+        <v>197.95312999999999</v>
       </c>
       <c r="J46">
-        <v>169.82051999999999</v>
+        <v>190.12020999999999</v>
       </c>
       <c r="K46">
-        <v>134.32982000000001</v>
+        <v>170.48435000000001</v>
       </c>
       <c r="L46">
-        <v>135.23766000000001</v>
+        <v>170.20402000000001</v>
       </c>
       <c r="M46">
-        <v>192.40432999999999</v>
+        <v>134.28889000000001</v>
       </c>
       <c r="N46">
-        <v>192.41533000000001</v>
+        <v>135.23397</v>
       </c>
       <c r="O46">
-        <v>212.95909</v>
+        <v>192.40346</v>
       </c>
       <c r="P46">
-        <v>318.60122000000001</v>
+        <v>192.40633</v>
       </c>
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.3">
@@ -3556,203 +3040,250 @@
         <v>3</v>
       </c>
       <c r="B47">
+        <v>171.75587999999999</v>
+      </c>
+      <c r="C47">
+        <v>243.62769</v>
+      </c>
+      <c r="D47">
         <v>147.14606000000001</v>
       </c>
-      <c r="C47">
-        <v>147.2647</v>
-      </c>
-      <c r="D47">
-        <v>158.17454000000001</v>
-      </c>
       <c r="E47">
-        <v>136.98324</v>
+        <v>146.33302</v>
       </c>
       <c r="F47">
+        <v>93.95993</v>
+      </c>
+      <c r="G47">
+        <v>118.16761</v>
+      </c>
+      <c r="H47">
         <v>139.65854999999999</v>
       </c>
-      <c r="G47">
-        <v>212.23553000000001</v>
-      </c>
-      <c r="H47">
-        <v>206.28527</v>
-      </c>
       <c r="I47">
-        <v>146.63256000000001</v>
+        <v>161.33551</v>
       </c>
       <c r="J47">
-        <v>145.77785</v>
+        <v>162.22132999999999</v>
       </c>
       <c r="K47">
-        <v>108.30021000000001</v>
+        <v>146.63321999999999</v>
       </c>
       <c r="L47">
-        <v>109.41844</v>
+        <v>146.24845999999999</v>
       </c>
       <c r="M47">
-        <v>166.51205999999999</v>
+        <v>108.27719999999999</v>
       </c>
       <c r="N47">
-        <v>166.52146999999999</v>
+        <v>109.41019</v>
       </c>
       <c r="O47">
-        <v>171.75587999999999</v>
+        <v>166.51213000000001</v>
       </c>
       <c r="P47">
-        <v>243.62769</v>
+        <v>166.51510999999999</v>
       </c>
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B48">
+      <c r="B48" s="4">
+        <v>-21.58962</v>
+      </c>
+      <c r="C48" s="4">
+        <v>114.60317999999999</v>
+      </c>
+      <c r="D48">
         <v>126.19732</v>
       </c>
-      <c r="C48">
-        <v>125.76322999999999</v>
-      </c>
-      <c r="D48" s="4">
-        <v>143.04382000000001</v>
-      </c>
-      <c r="E48" s="4">
-        <v>121.07324</v>
+      <c r="E48">
+        <v>120.12241</v>
       </c>
       <c r="F48" s="4">
+        <v>-3.59517</v>
+      </c>
+      <c r="G48" s="4">
+        <v>67.077839999999995</v>
+      </c>
+      <c r="H48" s="4">
         <v>103.47265</v>
       </c>
-      <c r="G48" s="4">
-        <v>163.89363</v>
-      </c>
-      <c r="H48" s="4">
-        <v>79.256469999999993</v>
-      </c>
       <c r="I48" s="4">
-        <v>138.22121999999999</v>
+        <v>42.454610000000002</v>
       </c>
       <c r="J48" s="4">
-        <v>137.58510000000001</v>
+        <v>66.138000000000005</v>
       </c>
       <c r="K48" s="4">
-        <v>81.11918</v>
+        <v>138.22123999999999</v>
       </c>
       <c r="L48" s="4">
-        <v>78.418340000000001</v>
+        <v>137.99950000000001</v>
       </c>
       <c r="M48" s="4">
-        <v>152.47541000000001</v>
+        <v>81.064179999999993</v>
       </c>
       <c r="N48" s="4">
-        <v>152.48998</v>
+        <v>78.408739999999995</v>
       </c>
       <c r="O48" s="4">
-        <v>-21.58962</v>
+        <v>152.47619</v>
       </c>
       <c r="P48" s="4">
-        <v>114.60317999999999</v>
+        <v>152.48262</v>
       </c>
     </row>
     <row r="49" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B49">
+      <c r="B49" s="4">
+        <v>3611.44</v>
+      </c>
+      <c r="C49" s="4">
+        <v>4944.59</v>
+      </c>
+      <c r="D49">
         <v>2551.36</v>
       </c>
-      <c r="C49">
-        <v>2600.5700000000002</v>
-      </c>
-      <c r="D49" s="4">
-        <v>2209.52</v>
-      </c>
-      <c r="E49" s="4">
-        <v>1800.66</v>
+      <c r="E49">
+        <v>2505.52</v>
       </c>
       <c r="F49" s="4">
+        <v>1369.11</v>
+      </c>
+      <c r="G49" s="4">
+        <v>1293.3499999999999</v>
+      </c>
+      <c r="H49" s="4">
         <v>1813.48</v>
       </c>
-      <c r="G49" s="4">
-        <v>3517.84</v>
-      </c>
-      <c r="H49" s="4">
-        <v>4427.2700000000004</v>
-      </c>
       <c r="I49" s="4">
-        <v>2238.3000000000002</v>
+        <v>2927.44</v>
       </c>
       <c r="J49" s="4">
-        <v>2224.7399999999998</v>
+        <v>3587.34</v>
       </c>
       <c r="K49" s="4">
-        <v>1553.7</v>
+        <v>2238.3200000000002</v>
       </c>
       <c r="L49" s="4">
-        <v>1536.23</v>
+        <v>2231.2199999999998</v>
       </c>
       <c r="M49" s="4">
-        <v>2539.71</v>
+        <v>1552.82</v>
       </c>
       <c r="N49" s="4">
-        <v>2540.04</v>
+        <v>1536.03</v>
       </c>
       <c r="O49" s="4">
-        <v>3611.44</v>
+        <v>2539.8000000000002</v>
       </c>
       <c r="P49" s="4">
-        <v>4944.59</v>
+        <v>2539.96</v>
       </c>
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A50" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B50">
+      <c r="B50" s="4">
+        <v>0.90874999999999995</v>
+      </c>
+      <c r="C50" s="4">
+        <v>1.28888</v>
+      </c>
+      <c r="D50">
         <v>0.77844999999999998</v>
       </c>
-      <c r="C50">
-        <v>0.77907999999999999</v>
-      </c>
-      <c r="D50" s="4">
-        <v>0.83679999999999999</v>
-      </c>
-      <c r="E50" s="4">
-        <v>0.72468999999999995</v>
+      <c r="E50">
+        <v>0.77415</v>
       </c>
       <c r="F50" s="4">
+        <v>0.49708000000000002</v>
+      </c>
+      <c r="G50" s="4">
+        <v>0.62514999999999998</v>
+      </c>
+      <c r="H50" s="4">
         <v>0.73884000000000005</v>
       </c>
-      <c r="G50" s="4">
-        <v>1.1228</v>
-      </c>
-      <c r="H50" s="4">
-        <v>1.0913200000000001</v>
-      </c>
       <c r="I50" s="4">
+        <v>0.85351999999999995</v>
+      </c>
+      <c r="J50" s="4">
+        <v>0.85821000000000003</v>
+      </c>
+      <c r="K50" s="4">
         <v>0.77573999999999999</v>
       </c>
-      <c r="J50" s="4">
-        <v>0.77122000000000002</v>
-      </c>
-      <c r="K50" s="4">
-        <v>0.57294999999999996</v>
-      </c>
       <c r="L50" s="4">
-        <v>0.57886000000000004</v>
+        <v>0.77371000000000001</v>
       </c>
       <c r="M50" s="4">
+        <v>0.57282</v>
+      </c>
+      <c r="N50" s="4">
+        <v>0.57882</v>
+      </c>
+      <c r="O50" s="4">
         <v>0.88090999999999997</v>
       </c>
-      <c r="N50" s="4">
-        <v>0.88095999999999997</v>
-      </c>
-      <c r="O50" s="4">
-        <v>0.90874999999999995</v>
-      </c>
       <c r="P50" s="4">
-        <v>1.28888</v>
+        <v>0.88092000000000004</v>
       </c>
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A51" s="2"/>
+      <c r="A51" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B51">
+        <v>0.69699999999999995</v>
+      </c>
+      <c r="C51">
+        <v>0.621</v>
+      </c>
+      <c r="D51">
+        <v>0.89600000000000002</v>
+      </c>
+      <c r="E51">
+        <v>0.88900000000000001</v>
+      </c>
+      <c r="F51">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="G51">
+        <v>0.89900000000000002</v>
+      </c>
+      <c r="H51">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="I51">
+        <v>0.70599999999999996</v>
+      </c>
+      <c r="J51">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="K51">
+        <v>0.92500000000000004</v>
+      </c>
+      <c r="L51">
+        <v>0.92600000000000005</v>
+      </c>
+      <c r="M51">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="N51">
+        <v>0.90700000000000003</v>
+      </c>
+      <c r="O51">
+        <v>0.91</v>
+      </c>
+      <c r="P51">
+        <v>0.91</v>
+      </c>
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A53" s="1" t="s">
@@ -3760,57 +3291,57 @@
       </c>
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="B54" s="2"/>
-      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A55" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B55">
-        <v>0.74770000000000003</v>
+        <v>0.39773999999999998</v>
       </c>
       <c r="C55">
-        <v>0.75163000000000002</v>
+        <v>0.52481</v>
       </c>
       <c r="D55">
-        <v>0.58492</v>
+        <v>0.73228000000000004</v>
       </c>
       <c r="E55">
-        <v>0.41288000000000002</v>
+        <v>0.75826000000000005</v>
       </c>
       <c r="F55">
+        <v>0.76070000000000004</v>
+      </c>
+      <c r="G55">
+        <v>0.53837000000000002</v>
+      </c>
+      <c r="H55">
         <v>0.65529999999999999</v>
       </c>
-      <c r="G55">
-        <v>0.54335</v>
-      </c>
-      <c r="H55">
-        <v>0.59891000000000005</v>
-      </c>
       <c r="I55">
+        <v>0.58901999999999999</v>
+      </c>
+      <c r="J55">
+        <v>0.52156999999999998</v>
+      </c>
+      <c r="K55">
         <v>0.79935999999999996</v>
       </c>
-      <c r="J55">
-        <v>0.79945999999999995</v>
-      </c>
-      <c r="K55">
+      <c r="L55">
+        <v>0.79952000000000001</v>
+      </c>
+      <c r="M55">
         <v>0.80700000000000005</v>
       </c>
-      <c r="L55">
+      <c r="N55">
         <v>0.80359999999999998</v>
       </c>
-      <c r="M55">
+      <c r="O55">
         <v>0.75239999999999996</v>
       </c>
-      <c r="N55">
+      <c r="P55">
         <v>0.75239999999999996</v>
-      </c>
-      <c r="O55">
-        <v>0.39773999999999998</v>
-      </c>
-      <c r="P55">
-        <v>0.52481</v>
       </c>
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.3">
@@ -3818,49 +3349,49 @@
         <v>2</v>
       </c>
       <c r="B56">
-        <v>236.16172</v>
+        <v>585.35820000000001</v>
       </c>
       <c r="C56">
-        <v>235.46485999999999</v>
+        <v>573.70992999999999</v>
       </c>
       <c r="D56">
-        <v>333.89425</v>
+        <v>242.02482000000001</v>
       </c>
       <c r="E56">
-        <v>927.00671</v>
+        <v>229.94092000000001</v>
       </c>
       <c r="F56">
+        <v>213.27456000000001</v>
+      </c>
+      <c r="G56">
+        <v>635.73617000000002</v>
+      </c>
+      <c r="H56">
         <v>248.72363000000001</v>
       </c>
-      <c r="G56">
-        <v>398.50585000000001</v>
-      </c>
-      <c r="H56">
-        <v>297.52821</v>
-      </c>
       <c r="I56">
-        <v>205.8837</v>
+        <v>366.65339999999998</v>
       </c>
       <c r="J56">
-        <v>205.83360999999999</v>
+        <v>362.61788999999999</v>
       </c>
       <c r="K56">
-        <v>209.02052</v>
+        <v>205.8836</v>
       </c>
       <c r="L56">
-        <v>209.27243999999999</v>
+        <v>205.78790000000001</v>
       </c>
       <c r="M56">
-        <v>235.66945999999999</v>
+        <v>209.01091</v>
       </c>
       <c r="N56">
-        <v>235.66676000000001</v>
+        <v>209.26209</v>
       </c>
       <c r="O56">
-        <v>585.35820000000001</v>
+        <v>235.66695000000001</v>
       </c>
       <c r="P56">
-        <v>573.70992999999999</v>
+        <v>235.66695999999999</v>
       </c>
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.3">
@@ -3868,49 +3399,49 @@
         <v>3</v>
       </c>
       <c r="B57">
-        <v>187.57248000000001</v>
+        <v>505.07920999999999</v>
       </c>
       <c r="C57">
-        <v>185.21116000000001</v>
+        <v>473.14111000000003</v>
       </c>
       <c r="D57">
-        <v>305.18646000000001</v>
+        <v>191.49608000000001</v>
       </c>
       <c r="E57">
-        <v>832.78224</v>
+        <v>179.16344000000001</v>
       </c>
       <c r="F57">
+        <v>177.58375000000001</v>
+      </c>
+      <c r="G57">
+        <v>530.17327</v>
+      </c>
+      <c r="H57">
         <v>195.94677999999999</v>
       </c>
-      <c r="G57">
-        <v>325.34257000000002</v>
-      </c>
-      <c r="H57">
-        <v>261.81279999999998</v>
-      </c>
       <c r="I57">
-        <v>170.17706999999999</v>
+        <v>275.63799999999998</v>
       </c>
       <c r="J57">
-        <v>170.17094</v>
+        <v>271.90397999999999</v>
       </c>
       <c r="K57">
-        <v>170.21517</v>
+        <v>170.17708999999999</v>
       </c>
       <c r="L57">
-        <v>169.66934000000001</v>
+        <v>170.17839000000001</v>
       </c>
       <c r="M57">
-        <v>188.99198000000001</v>
+        <v>170.30527000000001</v>
       </c>
       <c r="N57">
-        <v>188.98921000000001</v>
+        <v>169.65698</v>
       </c>
       <c r="O57">
-        <v>505.07920999999999</v>
+        <v>188.98991000000001</v>
       </c>
       <c r="P57">
-        <v>473.14111000000003</v>
+        <v>188.98993999999999</v>
       </c>
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.3">
@@ -3918,49 +3449,49 @@
         <v>4</v>
       </c>
       <c r="B58">
-        <v>5.0127600000000001</v>
+        <v>-375.16142000000002</v>
       </c>
       <c r="C58">
-        <v>-2.33636</v>
+        <v>-428.84949999999998</v>
       </c>
       <c r="D58">
-        <v>-235.74709999999999</v>
+        <v>0.81618999999999997</v>
       </c>
       <c r="E58">
-        <v>830.32428000000004</v>
+        <v>-2.1527699999999999</v>
       </c>
       <c r="F58">
+        <v>31.728860000000001</v>
+      </c>
+      <c r="G58">
+        <v>496.20735999999999</v>
+      </c>
+      <c r="H58">
         <v>67.338260000000005</v>
       </c>
-      <c r="G58">
-        <v>49.00179</v>
-      </c>
-      <c r="H58">
-        <v>-103.34376</v>
-      </c>
       <c r="I58">
-        <v>-4.3332600000000001</v>
+        <v>43.973669999999998</v>
       </c>
       <c r="J58">
-        <v>-4.5026299999999999</v>
+        <v>97.469229999999996</v>
       </c>
       <c r="K58">
-        <v>-36.702370000000002</v>
+        <v>-4.3337500000000002</v>
       </c>
       <c r="L58">
-        <v>-27.91563</v>
+        <v>-4.5582900000000004</v>
       </c>
       <c r="M58">
-        <v>-37.538170000000001</v>
+        <v>-36.732129999999998</v>
       </c>
       <c r="N58">
-        <v>-37.53633</v>
+        <v>-27.906330000000001</v>
       </c>
       <c r="O58">
-        <v>-375.16142000000002</v>
+        <v>-37.537050000000001</v>
       </c>
       <c r="P58">
-        <v>-428.84949999999998</v>
+        <v>-37.535240000000002</v>
       </c>
     </row>
     <row r="59" spans="1:16" ht="28.8" x14ac:dyDescent="0.3">
@@ -3968,49 +3499,49 @@
         <v>5</v>
       </c>
       <c r="B59">
-        <v>1673.83</v>
+        <v>8749.9599999999991</v>
       </c>
       <c r="C59">
-        <v>1480.84</v>
+        <v>8163.15</v>
       </c>
       <c r="D59">
-        <v>4920.72</v>
+        <v>1622</v>
       </c>
       <c r="E59">
-        <v>16096.96</v>
+        <v>1503.47</v>
       </c>
       <c r="F59">
+        <v>2995.72</v>
+      </c>
+      <c r="G59">
+        <v>10069.99</v>
+      </c>
+      <c r="H59">
         <v>2941.34</v>
       </c>
-      <c r="G59">
-        <v>4318.9399999999996</v>
-      </c>
-      <c r="H59">
-        <v>4677.43</v>
-      </c>
       <c r="I59">
-        <v>2375.2600000000002</v>
+        <v>5036.2299999999996</v>
       </c>
       <c r="J59">
-        <v>2378.8200000000002</v>
+        <v>3400.84</v>
       </c>
       <c r="K59">
-        <v>1819.68</v>
+        <v>2375.2800000000002</v>
       </c>
       <c r="L59">
-        <v>1632.16</v>
+        <v>2382.59</v>
       </c>
       <c r="M59">
-        <v>2419.5300000000002</v>
+        <v>1821.19</v>
       </c>
       <c r="N59">
-        <v>2419.44</v>
+        <v>1631.6</v>
       </c>
       <c r="O59">
-        <v>8749.9599999999991</v>
+        <v>2419.4699999999998</v>
       </c>
       <c r="P59">
-        <v>8163.15</v>
+        <v>2419.4699999999998</v>
       </c>
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.3">
@@ -4018,80 +3549,151 @@
         <v>30</v>
       </c>
       <c r="B60">
-        <v>0.85280999999999996</v>
+        <v>2.29637</v>
       </c>
       <c r="C60">
-        <v>0.84206999999999999</v>
+        <v>2.15116</v>
       </c>
       <c r="D60">
-        <v>1.3875500000000001</v>
+        <v>0.87065000000000003</v>
       </c>
       <c r="E60">
-        <v>3.7862900000000002</v>
+        <v>0.81457999999999997</v>
       </c>
       <c r="F60">
+        <v>0.80739000000000005</v>
+      </c>
+      <c r="G60">
+        <v>2.41046</v>
+      </c>
+      <c r="H60">
         <v>0.89088000000000001</v>
       </c>
-      <c r="G60">
-        <v>1.47919</v>
-      </c>
-      <c r="H60">
-        <v>1.19035</v>
-      </c>
       <c r="I60">
+        <v>1.2532000000000001</v>
+      </c>
+      <c r="J60">
+        <v>1.2362299999999999</v>
+      </c>
+      <c r="K60">
         <v>0.77371999999999996</v>
       </c>
-      <c r="J60">
-        <v>0.77368999999999999</v>
-      </c>
-      <c r="K60">
-        <v>0.77417000000000002</v>
-      </c>
       <c r="L60">
-        <v>0.77141000000000004</v>
+        <v>0.77373000000000003</v>
       </c>
       <c r="M60">
-        <v>0.85926000000000002</v>
+        <v>0.77429999999999999</v>
       </c>
       <c r="N60">
+        <v>0.77134999999999998</v>
+      </c>
+      <c r="O60">
         <v>0.85924999999999996</v>
       </c>
-      <c r="O60">
-        <v>2.29637</v>
-      </c>
       <c r="P60">
-        <v>2.15116</v>
+        <v>0.85924999999999996</v>
       </c>
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="A61" s="2"/>
+      <c r="A61" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61">
+        <v>0.11700000000000001</v>
+      </c>
+      <c r="C61">
+        <v>0.55100000000000005</v>
+      </c>
+      <c r="D61">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="E61">
+        <v>0.57099999999999995</v>
+      </c>
+      <c r="F61">
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="G61">
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="H61">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="I61">
+        <v>0.33400000000000002</v>
+      </c>
+      <c r="J61">
+        <v>0.188</v>
+      </c>
+      <c r="K61">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="L61">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="M61">
+        <v>0.65900000000000003</v>
+      </c>
+      <c r="N61">
+        <v>0.65200000000000002</v>
+      </c>
+      <c r="O61">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="P61">
+        <v>0.56499999999999995</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="B3:F3 H3:J3 L3:N3 P3:R3 T3:V3 X3:Z3 AB3:AD3">
+    <cfRule type="colorScale" priority="89">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:F4 H4:J4 L4:N4 P4:R4 T4:V4 X4:Z4 AB4:AD4">
+    <cfRule type="colorScale" priority="88">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF00B050"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B5:F5 H5:J5 L5:N5 P5:R5 T5:V5 X5:Z5 AB5:AD5">
     <cfRule type="colorScale" priority="87">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:F4 H4:J4 L4:N4 P4:R4 T4:V4 X4:Z4 AB4:AD4">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M4:N4 P4:R4 T4:V4 X4:Z4 AB4:AD4 I4:J4 E4:F4">
     <cfRule type="colorScale" priority="86">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF00B050"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFFF0000"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B5:F5 H5:J5 L5:N5 P5:R5 T5:V5 X5:Z5 AB5:AD5">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:F7 H7:J7 L7:N7 P7:R7 T7:V7 X7:Z7 AB7:AD7">
     <cfRule type="colorScale" priority="85">
       <colorScale>
         <cfvo type="min"/>
@@ -4103,19 +3705,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M4:N4 P4:R4 T4:V4 X4:Z4 AB4:AD4 I4:J4 E4:F4">
+  <conditionalFormatting sqref="B13:F13 H13:J13 L13:N13 P13:R13 T13:V13 X13:Z13 AB13:AD13">
     <cfRule type="colorScale" priority="84">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B7:F7 H7:J7 L7:N7 P7:R7 T7:V7 X7:Z7 AB7:AD7">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:F14 H14:J14 L14:N14 P14:R14 T14:V14 X14:Z14 AB14:AD14">
     <cfRule type="colorScale" priority="83">
       <colorScale>
         <cfvo type="min"/>
@@ -4127,19 +3729,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:F13 H13:J13 L13:N13 P13:R13 T13:V13 X13:Z13 AB13:AD13">
+  <conditionalFormatting sqref="B15:F15 H15:J15 L15:N15 P15:R15 T15:V15 X15:Z15 AB15:AD15">
     <cfRule type="colorScale" priority="82">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:F14 H14:J14 L14:N14 P14:R14 T14:V14 X14:Z14 AB14:AD14">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:F17 H17:J17 L17:N17 P17:R17 T17:V17 X17:Z17 AB17:AD17">
     <cfRule type="colorScale" priority="81">
       <colorScale>
         <cfvo type="min"/>
@@ -4151,7 +3753,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:F15 H15:J15 L15:N15 P15:R15 T15:V15 X15:Z15 AB15:AD15">
+  <conditionalFormatting sqref="B8:F8 H8:J8 L8:N8 P8:R8 T8:V8 X8:Z8 AB8:AD8">
     <cfRule type="colorScale" priority="80">
       <colorScale>
         <cfvo type="min"/>
@@ -4163,7 +3765,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:F17 H17:J17 L17:N17 P17:R17 T17:V17 X17:Z17 AB17:AD17">
+  <conditionalFormatting sqref="B18:F18 H18:J18 L18:N18 P18:R18 T18:V18 X18:Z18 AB18:AD18">
     <cfRule type="colorScale" priority="79">
       <colorScale>
         <cfvo type="min"/>
@@ -4175,19 +3777,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B8:F8 H8:J8 L8:N8 P8:R8 T8:V8 X8:Z8 AB8:AD8">
+  <conditionalFormatting sqref="B3:AE3">
     <cfRule type="colorScale" priority="78">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:F18 H18:J18 L18:N18 P18:R18 T18:V18 X18:Z18 AB18:AD18">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B4:AE4">
     <cfRule type="colorScale" priority="77">
       <colorScale>
         <cfvo type="min"/>
@@ -4199,19 +3801,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3:AE3">
+  <conditionalFormatting sqref="B5:AE5">
     <cfRule type="colorScale" priority="76">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B4:AE4">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B7:AE7">
     <cfRule type="colorScale" priority="75">
       <colorScale>
         <cfvo type="min"/>
@@ -4223,7 +3825,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5:AE5">
+  <conditionalFormatting sqref="B8:AE8">
     <cfRule type="colorScale" priority="74">
       <colorScale>
         <cfvo type="min"/>
@@ -4235,19 +3837,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B7:AE7">
+  <conditionalFormatting sqref="B13:AE13">
     <cfRule type="colorScale" priority="73">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B8:AE8">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:AE14">
     <cfRule type="colorScale" priority="72">
       <colorScale>
         <cfvo type="min"/>
@@ -4259,19 +3861,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13:AE13">
+  <conditionalFormatting sqref="B15:AE15">
     <cfRule type="colorScale" priority="71">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B14:AE14">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B17:AE17">
     <cfRule type="colorScale" priority="70">
       <colorScale>
         <cfvo type="min"/>
@@ -4283,7 +3885,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B15:AE15">
+  <conditionalFormatting sqref="B18:AE18">
     <cfRule type="colorScale" priority="69">
       <colorScale>
         <cfvo type="min"/>
@@ -4295,32 +3897,8 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B17:AE17">
-    <cfRule type="colorScale" priority="68">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B18:AE18">
-    <cfRule type="colorScale" priority="67">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
   <conditionalFormatting sqref="P30:AD30">
-    <cfRule type="colorScale" priority="62">
+    <cfRule type="colorScale" priority="64">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4332,7 +3910,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="P33:AD33">
-    <cfRule type="colorScale" priority="61">
+    <cfRule type="colorScale" priority="63">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
@@ -4344,18 +3922,42 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B25:P25">
+    <cfRule type="colorScale" priority="42">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B26:P26">
+    <cfRule type="colorScale" priority="41">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B27:P27">
     <cfRule type="colorScale" priority="40">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B26:P26">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B29:P29">
     <cfRule type="colorScale" priority="39">
       <colorScale>
         <cfvo type="min"/>
@@ -4367,7 +3969,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B27:P27">
+  <conditionalFormatting sqref="B30:O30">
     <cfRule type="colorScale" priority="38">
       <colorScale>
         <cfvo type="min"/>
@@ -4379,19 +3981,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:P29">
+  <conditionalFormatting sqref="B35:P35">
     <cfRule type="colorScale" priority="37">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B30:O30">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B36:P36">
     <cfRule type="colorScale" priority="36">
       <colorScale>
         <cfvo type="min"/>
@@ -4403,19 +4005,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B35:P35">
+  <conditionalFormatting sqref="O38:O40 B37:P37">
     <cfRule type="colorScale" priority="35">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B36:P36">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B39:N39 P39">
     <cfRule type="colorScale" priority="34">
       <colorScale>
         <cfvo type="min"/>
@@ -4427,7 +4029,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O38:O40 B37:P37">
+  <conditionalFormatting sqref="B40:N40 P40">
     <cfRule type="colorScale" priority="33">
       <colorScale>
         <cfvo type="min"/>
@@ -4439,63 +4041,63 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B39:N39 P39">
-    <cfRule type="colorScale" priority="32">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B40:N40 P40">
-    <cfRule type="colorScale" priority="31">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B6:AE6 B16:AE16 B38:N38 B28:P28 P38">
-    <cfRule type="expression" dxfId="95" priority="21">
+  <conditionalFormatting sqref="B6:AE6 B16:AE16 B38:N38 B28:P28 P38 B48:P48">
+    <cfRule type="expression" dxfId="11" priority="23">
       <formula>ABS(B6)&gt;300</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="94" priority="22">
+    <cfRule type="expression" dxfId="10" priority="24">
       <formula>AND(ABS(B6)&gt;150, ABS(B6)&lt;=200)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="93" priority="24">
+    <cfRule type="expression" dxfId="9" priority="26">
       <formula>AND(ABS(B6)&gt;50, ABS(B6)&lt;=100)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="92" priority="25">
+    <cfRule type="expression" dxfId="8" priority="27">
       <formula>AND(ABS(B6)&gt;200, ABS(B6)&lt;=300)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="91" priority="26">
+    <cfRule type="expression" dxfId="7" priority="28">
       <formula>AND(ABS(B6)&gt;100, ABS(B6)&lt;=150)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="90" priority="27">
+    <cfRule type="expression" dxfId="6" priority="29">
       <formula>AND(ABS(B6)&gt;0, ABS(B6)&lt;=50)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="P50">
+  <conditionalFormatting sqref="C50">
+    <cfRule type="colorScale" priority="22">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C53">
+    <cfRule type="colorScale" priority="21">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B45:P45">
     <cfRule type="colorScale" priority="20">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="P53">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B46:P46">
     <cfRule type="colorScale" priority="19">
       <colorScale>
         <cfvo type="min"/>
@@ -4507,19 +4109,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B45:P45">
+  <conditionalFormatting sqref="B47:P47">
     <cfRule type="colorScale" priority="18">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B46:P46">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B49:P49">
     <cfRule type="colorScale" priority="17">
       <colorScale>
         <cfvo type="min"/>
@@ -4531,7 +4133,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B47:P47">
+  <conditionalFormatting sqref="D50:P50 B50">
     <cfRule type="colorScale" priority="16">
       <colorScale>
         <cfvo type="min"/>
@@ -4543,19 +4145,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B49:P49">
+  <conditionalFormatting sqref="B55:P55">
     <cfRule type="colorScale" priority="15">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B50:O50">
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B56:P56">
     <cfRule type="colorScale" priority="14">
       <colorScale>
         <cfvo type="min"/>
@@ -4567,19 +4169,19 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B55:P55">
+  <conditionalFormatting sqref="B58:B60 B57:P57">
     <cfRule type="colorScale" priority="13">
       <colorScale>
         <cfvo type="min"/>
         <cfvo type="percentile" val="50"/>
         <cfvo type="max"/>
-        <color rgb="FFF8696B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FF63BE7B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B56:P56">
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C59:P59">
     <cfRule type="colorScale" priority="12">
       <colorScale>
         <cfvo type="min"/>
@@ -4591,7 +4193,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="O58:O60 B57:P57">
+  <conditionalFormatting sqref="C60:P60">
     <cfRule type="colorScale" priority="11">
       <colorScale>
         <cfvo type="min"/>
@@ -4603,48 +4205,24 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B59:N59 P59">
-    <cfRule type="colorScale" priority="10">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B60:N60 P60">
-    <cfRule type="colorScale" priority="9">
-      <colorScale>
-        <cfvo type="min"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="max"/>
-        <color rgb="FF63BE7B"/>
-        <color rgb="FFFFEB84"/>
-        <color rgb="FFF8696B"/>
-      </colorScale>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B58:N58 B48:P48 P58">
-    <cfRule type="expression" dxfId="89" priority="3">
-      <formula>ABS(B48)&gt;300</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="88" priority="4">
-      <formula>AND(ABS(B48)&gt;150, ABS(B48)&lt;=200)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="87" priority="5">
-      <formula>AND(ABS(B48)&gt;50, ABS(B48)&lt;=100)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="86" priority="6">
-      <formula>AND(ABS(B48)&gt;200, ABS(B48)&lt;=300)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="85" priority="7">
-      <formula>AND(ABS(B48)&gt;100, ABS(B48)&lt;=150)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="84" priority="8">
-      <formula>AND(ABS(B48)&gt;0, ABS(B48)&lt;=50)</formula>
+  <conditionalFormatting sqref="C58:P58">
+    <cfRule type="expression" dxfId="5" priority="5">
+      <formula>ABS(C58)&gt;300</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>AND(ABS(C58)&gt;150, ABS(C58)&lt;=200)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="7">
+      <formula>AND(ABS(C58)&gt;50, ABS(C58)&lt;=100)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="8">
+      <formula>AND(ABS(C58)&gt;200, ABS(C58)&lt;=300)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="9">
+      <formula>AND(ABS(C58)&gt;100, ABS(C58)&lt;=150)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="10">
+      <formula>AND(ABS(C58)&gt;0, ABS(C58)&lt;=50)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B51:P51">
@@ -4680,7 +4258,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D7965FB-BEA3-4857-9385-996B228DED8D}">
   <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
@@ -5769,22 +5347,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:C6 C16">
-    <cfRule type="expression" dxfId="47" priority="73">
+    <cfRule type="expression" dxfId="35" priority="73">
       <formula>ABS(B6)&gt;300</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="46" priority="74">
+    <cfRule type="expression" dxfId="34" priority="74">
       <formula>AND(ABS(B6)&gt;150, ABS(B6)&lt;=200)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="45" priority="75">
+    <cfRule type="expression" dxfId="33" priority="75">
       <formula>AND(ABS(B6)&gt;50, ABS(B6)&lt;=100)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="44" priority="76">
+    <cfRule type="expression" dxfId="32" priority="76">
       <formula>AND(ABS(B6)&gt;200, ABS(B6)&lt;=300)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="43" priority="77">
+    <cfRule type="expression" dxfId="31" priority="77">
       <formula>AND(ABS(B6)&gt;100, ABS(B6)&lt;=150)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="42" priority="78">
+    <cfRule type="expression" dxfId="30" priority="78">
       <formula>AND(ABS(B6)&gt;0, ABS(B6)&lt;=50)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5969,22 +5547,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B6:J6 B16:J16">
-    <cfRule type="expression" dxfId="41" priority="57">
+    <cfRule type="expression" dxfId="29" priority="57">
       <formula>ABS(B6)&gt;300</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="40" priority="59">
+    <cfRule type="expression" dxfId="28" priority="58">
+      <formula>AND(ABS(B6)&gt;150, ABS(B6)&lt;=200)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="27" priority="59">
       <formula>AND(ABS(B6)&gt;50, ABS(B6)&lt;=100)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="39" priority="58">
-      <formula>AND(ABS(B6)&gt;150, ABS(B6)&lt;=200)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="38" priority="60">
+    <cfRule type="expression" dxfId="26" priority="60">
       <formula>AND(ABS(B6)&gt;200, ABS(B6)&lt;=300)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="37" priority="61">
+    <cfRule type="expression" dxfId="25" priority="61">
       <formula>AND(ABS(B6)&gt;100, ABS(B6)&lt;=150)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="62">
+    <cfRule type="expression" dxfId="24" priority="62">
       <formula>AND(ABS(B6)&gt;0, ABS(B6)&lt;=50)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6193,22 +5771,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:C26 C36">
-    <cfRule type="expression" dxfId="35" priority="29">
+    <cfRule type="expression" dxfId="23" priority="29">
       <formula>ABS(B26)&gt;300</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="30">
+    <cfRule type="expression" dxfId="22" priority="30">
       <formula>AND(ABS(B26)&gt;150, ABS(B26)&lt;=200)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="31">
+    <cfRule type="expression" dxfId="21" priority="31">
       <formula>AND(ABS(B26)&gt;50, ABS(B26)&lt;=100)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="32">
+    <cfRule type="expression" dxfId="20" priority="32">
       <formula>AND(ABS(B26)&gt;200, ABS(B26)&lt;=300)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="33">
+    <cfRule type="expression" dxfId="19" priority="33">
       <formula>AND(ABS(B26)&gt;100, ABS(B26)&lt;=150)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="34">
+    <cfRule type="expression" dxfId="18" priority="34">
       <formula>AND(ABS(B26)&gt;0, ABS(B26)&lt;=50)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6393,22 +5971,22 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="B26:J26 B36:J36">
-    <cfRule type="expression" dxfId="29" priority="13">
+    <cfRule type="expression" dxfId="17" priority="13">
       <formula>ABS(B26)&gt;300</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="14">
+    <cfRule type="expression" dxfId="16" priority="14">
       <formula>AND(ABS(B26)&gt;150, ABS(B26)&lt;=200)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="15">
+    <cfRule type="expression" dxfId="15" priority="15">
       <formula>AND(ABS(B26)&gt;50, ABS(B26)&lt;=100)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="16">
+    <cfRule type="expression" dxfId="14" priority="16">
       <formula>AND(ABS(B26)&gt;200, ABS(B26)&lt;=300)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="17">
+    <cfRule type="expression" dxfId="13" priority="17">
       <formula>AND(ABS(B26)&gt;100, ABS(B26)&lt;=150)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="24" priority="18">
+    <cfRule type="expression" dxfId="12" priority="18">
       <formula>AND(ABS(B26)&gt;0, ABS(B26)&lt;=50)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>